<commit_message>
feat: Update email automation to use new 'We help companies better leverage digital and technology' template and add associated message files.
</commit_message>
<xml_diff>
--- a/Test Mail.xlsx
+++ b/Test Mail.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,11 +461,11 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45980</v>
+        <v>46000</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Not Sent: Date passed (2025-11-19)</t>
+          <t>Sent at 2025-12-09 15:37:14</t>
         </is>
       </c>
     </row>
@@ -476,26 +476,11 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45981</v>
+        <v>46000</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Sent at 2025-11-20 20:31:11</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>gokuldaskannadas@gmail.com</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>45982</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Sent at 2025-11-21 09:18:16</t>
+          <t>Sent at 2025-12-09 15:37:16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add configuration for email sending with templates
- Introduced configuration variables for Excel file and template directory.
- Defined columns for email IDs and template names to streamline email generation process.
</commit_message>
<xml_diff>
--- a/Test Mail.xlsx
+++ b/Test Mail.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,6 +453,11 @@
           <t>Status</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Templates</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -461,11 +466,16 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46000</v>
+        <v>46020</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sent at 2025-12-09 15:37:14</t>
+          <t>Sent at 2025-12-29 11:59:21</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Customer Mail New.msg</t>
         </is>
       </c>
     </row>
@@ -476,11 +486,16 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>46000</v>
+        <v>46020</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Sent at 2025-12-09 15:37:16</t>
+          <t>Sent at 2025-12-29 11:59:23</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Power BI.msg</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Add new 'Power BI' and 'Customer Mail New' email templates and update test data for automation.
</commit_message>
<xml_diff>
--- a/Test Mail.xlsx
+++ b/Test Mail.xlsx
@@ -20,16 +20,13 @@
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -40,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -48,21 +45,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -438,22 +426,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Mail ID</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Templates</t>
         </is>
@@ -462,15 +450,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>rajan@finlytyx.com</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>46020</v>
+          <t>adil@finlytyx.com</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>46056</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sent at 2025-12-29 11:59:21</t>
+          <t>Sent at 2026-02-03 17:09:30</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -482,15 +470,15 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>gokuldas@finlytyx.com</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>46020</v>
+          <t>mashal@finlytyx.com</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>46056</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Sent at 2025-12-29 11:59:23</t>
+          <t>Sent at 2026-02-03 17:09:32</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">

</xml_diff>